<commit_message>
folders gemaakt en classes
</commit_message>
<xml_diff>
--- a/Map1.xlsx
+++ b/Map1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
   <si>
     <t>dag</t>
   </si>
@@ -139,6 +139,27 @@
   </si>
   <si>
     <t xml:space="preserve">database fotosjaak geëxporteerd </t>
+  </si>
+  <si>
+    <t>folder class gemaakt in de working directory</t>
+  </si>
+  <si>
+    <t>folder cconfig gemaakt</t>
+  </si>
+  <si>
+    <t>velden gedefined</t>
+  </si>
+  <si>
+    <t>database geselecteerd</t>
+  </si>
+  <si>
+    <t>or die erbij gemaakt</t>
+  </si>
+  <si>
+    <t>commentaar erbij gezet</t>
+  </si>
+  <si>
+    <t>git bijgewerkt</t>
   </si>
 </sst>
 </file>
@@ -538,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,7 +640,7 @@
         <v>0.36458333333333331</v>
       </c>
       <c r="D8" s="2">
-        <v>0.38541666666666669</v>
+        <v>0.40069444444444446</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -629,13 +650,17 @@
       </c>
       <c r="H8" s="2">
         <f>D8-C8</f>
-        <v>2.083333333333337E-2</v>
+        <v>3.6111111111111149E-2</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="C9" s="2">
+        <v>0.40069444444444446</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.42083333333333334</v>
+      </c>
       <c r="E9">
         <v>2</v>
       </c>
@@ -643,14 +668,18 @@
         <v>37</v>
       </c>
       <c r="H9" s="2">
-        <f t="shared" ref="H9:H30" si="0">D9-C9</f>
-        <v>0</v>
+        <f t="shared" ref="H9:H18" si="0">D9-C9</f>
+        <v>2.0138888888888873E-2</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="C10" s="2">
+        <v>0.42083333333333334</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.43055555555555558</v>
+      </c>
       <c r="E10">
         <v>3</v>
       </c>
@@ -659,13 +688,17 @@
       </c>
       <c r="H10" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9.7222222222222432E-3</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="C11" s="2">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.45833333333333331</v>
+      </c>
       <c r="E11">
         <v>4</v>
       </c>
@@ -674,177 +707,190 @@
       </c>
       <c r="H11" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.7777777777777735E-2</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="C12" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.47013888888888888</v>
+      </c>
       <c r="E12">
         <v>5</v>
       </c>
+      <c r="F12" t="s">
+        <v>40</v>
+      </c>
       <c r="H12" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.1805555555555569E-2</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="C13" s="2">
+        <v>0.47013888888888888</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="E13">
+        <v>6</v>
+      </c>
+      <c r="F13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="0"/>
+        <v>2.0833333333333814E-3</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="C14" s="2">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="E14">
+        <v>7</v>
+      </c>
+      <c r="F14" t="s">
+        <v>42</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="0"/>
+        <v>6.9444444444444198E-3</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="C15" s="2">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="E15">
+        <v>8</v>
+      </c>
+      <c r="F15" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="0"/>
+        <v>1.7361111111111049E-2</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="C16" s="2">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.4909722222222222</v>
+      </c>
+      <c r="E16">
+        <v>9</v>
+      </c>
+      <c r="F16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="0"/>
+        <v>1.388888888888884E-3</v>
+      </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="H17" s="2"/>
+      <c r="C17" s="2">
+        <v>0.4909722222222222</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="E17">
+        <v>10</v>
+      </c>
+      <c r="F17" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="0"/>
+        <v>2.0833333333333814E-3</v>
+      </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="H18" s="2"/>
+      <c r="C18" s="2">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E18">
+        <v>11</v>
+      </c>
+      <c r="F18" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" si="0"/>
+        <v>6.9444444444444198E-3</v>
+      </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
-      <c r="E19">
-        <v>6</v>
-      </c>
-      <c r="H19" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="H19" s="2"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
-      <c r="E20">
-        <v>7</v>
-      </c>
-      <c r="H20" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="H20" s="2"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21">
-        <v>8</v>
-      </c>
-      <c r="H21" s="2">
-        <f>D21-C21</f>
-        <v>0</v>
-      </c>
+      <c r="H21" s="2"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-      <c r="E22">
-        <v>9</v>
-      </c>
-      <c r="H22" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="H22" s="2"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
-      <c r="E23">
-        <v>10</v>
-      </c>
-      <c r="H23" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="H23" s="2"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
-      <c r="E24">
-        <v>11</v>
-      </c>
-      <c r="H24" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="H24" s="2"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E25">
-        <v>12</v>
-      </c>
-      <c r="H25" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="H25" s="2"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E26">
-        <v>13</v>
-      </c>
-      <c r="H26" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="H26" s="2"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E27">
-        <v>14</v>
-      </c>
-      <c r="H27" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="H27" s="2"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E28">
-        <v>15</v>
-      </c>
-      <c r="H28" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="H28" s="2"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E29">
-        <v>16</v>
-      </c>
-      <c r="H29" s="2">
-        <f>D29-C29</f>
-        <v>0</v>
-      </c>
+      <c r="H29" s="2"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E30">
-        <v>17</v>
-      </c>
-      <c r="H30" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="H30" s="2"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
@@ -852,7 +898,7 @@
       </c>
       <c r="H31" s="2">
         <f>SUM(H8:H30)</f>
-        <v>2.083333333333337E-2</v>
+        <v>0.1423611111111111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
logboek bijgewerkt, een fire query toegevoegd
</commit_message>
<xml_diff>
--- a/Map1.xlsx
+++ b/Map1.xlsx
@@ -4,22 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Blad2" sheetId="2" state="hidden" r:id="rId1"/>
     <sheet name="Blad3" sheetId="3" state="hidden" r:id="rId2"/>
     <sheet name="Blad5" sheetId="5" state="hidden" r:id="rId3"/>
     <sheet name="weeknr 48web" sheetId="9" r:id="rId4"/>
-    <sheet name="weeknr 48" sheetId="8" r:id="rId5"/>
-    <sheet name="totaal" sheetId="6" r:id="rId6"/>
+    <sheet name="weeknr 48game" sheetId="8" r:id="rId5"/>
+    <sheet name="weeknr 49game" sheetId="10" r:id="rId6"/>
+    <sheet name="totaal" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="59">
   <si>
     <t>dag</t>
   </si>
@@ -160,6 +161,42 @@
   </si>
   <si>
     <t>git bijgewerkt</t>
+  </si>
+  <si>
+    <t>48 web</t>
+  </si>
+  <si>
+    <t>48 game</t>
+  </si>
+  <si>
+    <t>Instantie/Object gemaakt van het type startscene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">draw methode gemaakt </t>
+  </si>
+  <si>
+    <t>startscene draw afgemaakt, en een kleurtje gegeven</t>
+  </si>
+  <si>
+    <t>play,help,gameover scenes gemaakt</t>
+  </si>
+  <si>
+    <t>gameTime toegevoegd</t>
+  </si>
+  <si>
+    <t>Iscene toegevoegd, library's aangepast</t>
+  </si>
+  <si>
+    <t>static input class gemaakt</t>
+  </si>
+  <si>
+    <t>is key down gedefineerd</t>
+  </si>
+  <si>
+    <t>is key up gedefineerd</t>
+  </si>
+  <si>
+    <t>commit gemaakt lokaal</t>
   </si>
 </sst>
 </file>
@@ -559,7 +596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -911,7 +948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -1297,10 +1334,394 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:H31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="8" customWidth="1"/>
+    <col min="5" max="5" width="4.28515625" customWidth="1"/>
+    <col min="6" max="6" width="38.140625" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1">
+        <v>41603</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="2">
+        <f>D8-C8</f>
+        <v>1.0416666666666685E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+      <c r="C9" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" ref="H9:H30" si="0">D9-C9</f>
+        <v>1.0416666666666685E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="C10" s="2">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="0"/>
+        <v>6.9444444444444198E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="C11" s="2">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.41319444444444442</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="0"/>
+        <v>2.0833333333333315E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" s="2">
+        <v>0.41319444444444442</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="0"/>
+        <v>3.4722222222222654E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="H13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="E19">
+        <v>6</v>
+      </c>
+      <c r="F19" t="s">
+        <v>54</v>
+      </c>
+      <c r="H19" s="2">
+        <f t="shared" si="0"/>
+        <v>1.041666666666663E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C20" s="2">
+        <v>0.4375</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E20">
+        <v>7</v>
+      </c>
+      <c r="F20" t="s">
+        <v>55</v>
+      </c>
+      <c r="H20" s="2">
+        <f t="shared" si="0"/>
+        <v>2.0833333333333315E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C21" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="E21">
+        <v>8</v>
+      </c>
+      <c r="F21" t="s">
+        <v>56</v>
+      </c>
+      <c r="H21" s="2">
+        <f>D21-C21</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C22" s="2">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="E22">
+        <v>9</v>
+      </c>
+      <c r="F22" t="s">
+        <v>57</v>
+      </c>
+      <c r="H22" s="2">
+        <f t="shared" si="0"/>
+        <v>1.041666666666663E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C23" s="8">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D23" s="8">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E23">
+        <v>10</v>
+      </c>
+      <c r="F23" t="s">
+        <v>58</v>
+      </c>
+      <c r="H23" s="2">
+        <f t="shared" si="0"/>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24">
+        <v>11</v>
+      </c>
+      <c r="H24" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>12</v>
+      </c>
+      <c r="H25" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>13</v>
+      </c>
+      <c r="H26" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>14</v>
+      </c>
+      <c r="H27" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>15</v>
+      </c>
+      <c r="H28" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>16</v>
+      </c>
+      <c r="H29" s="2">
+        <f>D29-C29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <v>17</v>
+      </c>
+      <c r="H30" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>5</v>
+      </c>
+      <c r="H31" s="2">
+        <f>SUM(H8:H30)</f>
+        <v>0.17708333333333331</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1349,24 +1770,34 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="2">
+        <f>'weeknr 48web'!H31</f>
+        <v>0.1423611111111111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="2">
-        <f>'weeknr 48'!H31</f>
+      <c r="B8" s="2">
+        <f>'weeknr 48game'!H31</f>
         <v>0.18680555555555567</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-    </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4"/>
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B10" s="7">
         <f>SUM(B7:B8)</f>
-        <v>0.18680555555555567</v>
+        <v>0.32916666666666677</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
login tabel gemaakt en nog meer
</commit_message>
<xml_diff>
--- a/Map1.xlsx
+++ b/Map1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Blad2" sheetId="2" state="hidden" r:id="rId1"/>
@@ -13,14 +13,15 @@
     <sheet name="weeknr 48web" sheetId="9" r:id="rId4"/>
     <sheet name="weeknr 48game" sheetId="8" r:id="rId5"/>
     <sheet name="weeknr 49game" sheetId="10" r:id="rId6"/>
-    <sheet name="totaal" sheetId="6" r:id="rId7"/>
+    <sheet name="weeknr 49web" sheetId="12" r:id="rId7"/>
+    <sheet name="totaal" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="61">
   <si>
     <t>dag</t>
   </si>
@@ -197,6 +198,12 @@
   </si>
   <si>
     <t>commit gemaakt lokaal</t>
+  </si>
+  <si>
+    <t>49 web</t>
+  </si>
+  <si>
+    <t>aptana, wamp opstarten</t>
   </si>
 </sst>
 </file>
@@ -1336,8 +1343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1411,7 +1418,7 @@
         <v>24</v>
       </c>
       <c r="B8" s="1">
-        <v>41603</v>
+        <v>41610</v>
       </c>
       <c r="C8" s="2">
         <v>0.36458333333333331</v>
@@ -1718,10 +1725,292 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="8" customWidth="1"/>
+    <col min="5" max="5" width="4.28515625" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1">
+        <v>41610</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.61319444444444449</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H8" s="2">
+        <f>D8-C8</f>
+        <v>4.8611111111110938E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" ref="H9:H18" si="0">D9-C9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13">
+        <v>6</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14">
+        <v>7</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15">
+        <v>8</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16">
+        <v>9</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17">
+        <v>10</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18">
+        <v>11</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>5</v>
+      </c>
+      <c r="H31" s="2">
+        <f>SUM(H8:H30)</f>
+        <v>4.8611111111110938E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1788,8 +2077,13 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="2"/>
+      <c r="A9" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="2">
+        <f>'weeknr 49web'!H31</f>
+        <v>4.8611111111110938E-3</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">

</xml_diff>

<commit_message>
toets gemaakt commit gemaakt
</commit_message>
<xml_diff>
--- a/Map1.xlsx
+++ b/Map1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" firstSheet="10" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Blad2" sheetId="2" state="hidden" r:id="rId1"/>
@@ -14,14 +14,18 @@
     <sheet name="weeknr 48game" sheetId="8" r:id="rId5"/>
     <sheet name="weeknr 49game" sheetId="10" r:id="rId6"/>
     <sheet name="weeknr 49web" sheetId="12" r:id="rId7"/>
-    <sheet name="totaal" sheetId="6" r:id="rId8"/>
+    <sheet name="weeknr 50game" sheetId="13" r:id="rId8"/>
+    <sheet name="weeknr 50web" sheetId="14" r:id="rId9"/>
+    <sheet name="totaal" sheetId="6" r:id="rId10"/>
+    <sheet name="Toets1 GameScene" sheetId="15" r:id="rId11"/>
+    <sheet name="Blad1" sheetId="16" r:id="rId12"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="93">
   <si>
     <t>dag</t>
   </si>
@@ -204,6 +208,102 @@
   </si>
   <si>
     <t>aptana, wamp opstarten</t>
+  </si>
+  <si>
+    <t>visual studio opgestart en de rest nagekeken op eventuele fouten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nieuwe class image gemaakt in de map HelperClass </t>
+  </si>
+  <si>
+    <t>instanties gemaakt van background en title</t>
+  </si>
+  <si>
+    <t>in de startscene class roept de constructor de initalize methode aan en zo verder</t>
+  </si>
+  <si>
+    <t>de image constructor gemaakt en de argumenten erbij gezet.</t>
+  </si>
+  <si>
+    <t>rectangle aangemaakt in de image class en in de constructor</t>
+  </si>
+  <si>
+    <t>buttons toegevoegd</t>
+  </si>
+  <si>
+    <t>color toegevoegd, nu kan elk knopje een andere kleur.</t>
+  </si>
+  <si>
+    <t>enum gemaakt voor het uitlezen van welk knopje er is ingedrukt.</t>
+  </si>
+  <si>
+    <t>switch case gemaakt</t>
+  </si>
+  <si>
+    <t>wamp opstarten enzo</t>
+  </si>
+  <si>
+    <t>Logboek</t>
+  </si>
+  <si>
+    <t>Pyramid Panic</t>
+  </si>
+  <si>
+    <t>Arjan de Ruijter</t>
+  </si>
+  <si>
+    <t>Toets 1 GameScenes</t>
+  </si>
+  <si>
+    <t>maandag</t>
+  </si>
+  <si>
+    <t>Maak een commit met naam: Toets1 commit 2</t>
+  </si>
+  <si>
+    <t>Maak in de AnimatedSprite class een field: private Vector2 pivot</t>
+  </si>
+  <si>
+    <t>Geef this.pivot in de constructor van de AnimatedSprite class de waarde new Vector2(16f, 16)</t>
+  </si>
+  <si>
+    <t>Verander in de Draw method in de AnimatedSprite class het argument origin van Vector2.Zero naar this.pivot</t>
+  </si>
+  <si>
+    <t>Verander de grenswaarden van de omkeerpunten van de beetles zodat ze niet buiten het scherm komen en niet eerder omkeren.</t>
+  </si>
+  <si>
+    <t>Verander de grenswaarden van de omkeerpunten van de scorpions zodat ze niet buiten het scherm komen en niet eerder omkeren.</t>
+  </si>
+  <si>
+    <t>Maak een commit genaamd: "Draaipunt verandert van de Draw method in AnimatedSprite class"</t>
+  </si>
+  <si>
+    <t>Webapplicatie van fotosjaak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opdracht: Maak een nieuwe gebruikersrol coworker en zorg dat deze kan inloggen in de database </t>
+  </si>
+  <si>
+    <t>dinsdag</t>
+  </si>
+  <si>
+    <t>Maak een nieuwe gebruikersrol coworker aan in de database.</t>
+  </si>
+  <si>
+    <t>Maak een nieuwe homepage genaamd coworker_homepage.php aan</t>
+  </si>
+  <si>
+    <t>voeg bij de pagina checklogin.php de nieuw gebruikersrol toe zodat een coworker die inlogt naar coworker_homepage wordt gestuurd.</t>
+  </si>
+  <si>
+    <t>Maak een nieuwe gebruiker aan.</t>
+  </si>
+  <si>
+    <t>Verander in de database handmatig zijn gebruikersrol van customer naar coworker.</t>
+  </si>
+  <si>
+    <t>Log in als de nieuwe gebruiker.</t>
   </si>
 </sst>
 </file>
@@ -215,7 +315,7 @@
     <numFmt numFmtId="165" formatCode="h:mm;@"/>
     <numFmt numFmtId="166" formatCode="[h]:mm:ss;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,6 +330,27 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -249,10 +370,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -264,9 +386,106 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -575,6 +794,726 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="44.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="5"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="2">
+        <f>'weeknr 48web'!H31</f>
+        <v>0.1423611111111111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="2">
+        <f>'weeknr 48game'!H31</f>
+        <v>0.18680555555555567</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="2">
+        <f>'weeknr 49web'!H31</f>
+        <v>4.8611111111110938E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="7">
+        <f>SUM(B7:B8)</f>
+        <v>0.32916666666666677</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="20"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="29">
+        <v>41666</v>
+      </c>
+      <c r="C7" s="30">
+        <v>0.37847222222222227</v>
+      </c>
+      <c r="D7" s="30">
+        <v>0.37916666666666671</v>
+      </c>
+      <c r="E7" s="28">
+        <v>1</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="G7" s="30">
+        <v>6.9444444444444198E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="28"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="30">
+        <v>0.37986111111111115</v>
+      </c>
+      <c r="D8" s="30">
+        <v>0.38055555555555559</v>
+      </c>
+      <c r="E8" s="28">
+        <v>2</v>
+      </c>
+      <c r="F8" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" s="30">
+        <v>6.9444444444444198E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="28"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="30">
+        <v>0.38125000000000003</v>
+      </c>
+      <c r="D9" s="30">
+        <v>0.38194444444444448</v>
+      </c>
+      <c r="E9" s="28">
+        <v>3</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="G9" s="30">
+        <v>6.9444444444444198E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30">
+        <v>0.38263888888888892</v>
+      </c>
+      <c r="D10" s="30">
+        <v>0.38333333333333336</v>
+      </c>
+      <c r="E10" s="28">
+        <v>4</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="G10" s="30">
+        <v>6.9444444444444198E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="30">
+        <v>0.3840277777777778</v>
+      </c>
+      <c r="D11" s="30">
+        <v>0.38472222222222224</v>
+      </c>
+      <c r="E11" s="28">
+        <v>5</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="G11" s="30">
+        <v>6.9444444444444198E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="30">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="D12" s="30">
+        <v>0.38611111111111113</v>
+      </c>
+      <c r="E12" s="28">
+        <v>6</v>
+      </c>
+      <c r="F12" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="G12" s="30">
+        <v>6.9444444444444198E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="30">
+        <v>0.38680555555555557</v>
+      </c>
+      <c r="D13" s="30">
+        <v>0.38750000000000001</v>
+      </c>
+      <c r="E13" s="28">
+        <v>7</v>
+      </c>
+      <c r="F13" s="31"/>
+      <c r="G13" s="30">
+        <v>6.9444444444444198E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="28"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="30">
+        <v>0.38819444444444445</v>
+      </c>
+      <c r="D14" s="30">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="E14" s="28">
+        <v>8</v>
+      </c>
+      <c r="F14" s="31"/>
+      <c r="G14" s="30">
+        <v>6.9444444444444198E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="28"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" s="30">
+        <v>5.5555555555555358E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="23"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="25"/>
+    </row>
+    <row r="17" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="12">
+        <v>0.59444444444444444</v>
+      </c>
+      <c r="D17" s="12">
+        <v>0.59444444444444444</v>
+      </c>
+      <c r="E17" s="18">
+        <v>11</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="G17" s="12">
+        <f t="shared" ref="G17" si="0">D17-C17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="12">
+        <f>SUM(G7:G16)</f>
+        <v>1.1111111111111072E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="42.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="G1" s="35"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" s="35"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="35"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="38">
+        <v>41667</v>
+      </c>
+      <c r="C7" s="39">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="D7" s="39">
+        <f>C7+TIME(0,1,0)</f>
+        <v>0.36527777777777776</v>
+      </c>
+      <c r="E7" s="37">
+        <v>1</v>
+      </c>
+      <c r="F7" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="G7" s="41">
+        <f t="shared" ref="G7:G18" si="0">D7-C7</f>
+        <v>6.9444444444444198E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="37"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="39">
+        <f>D7+TIME(0,1,0)</f>
+        <v>0.3659722222222222</v>
+      </c>
+      <c r="D8" s="39">
+        <f t="shared" ref="D8:D18" si="1">C8+TIME(0,1,0)</f>
+        <v>0.36666666666666664</v>
+      </c>
+      <c r="E8" s="37">
+        <v>2</v>
+      </c>
+      <c r="F8" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="G8" s="41">
+        <f t="shared" si="0"/>
+        <v>6.9444444444444198E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="37"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="39">
+        <f t="shared" ref="C9:C18" si="2">D8+TIME(0,1,0)</f>
+        <v>0.36736111111111108</v>
+      </c>
+      <c r="D9" s="39">
+        <f t="shared" si="1"/>
+        <v>0.36805555555555552</v>
+      </c>
+      <c r="E9" s="37">
+        <v>3</v>
+      </c>
+      <c r="F9" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="G9" s="41">
+        <f t="shared" si="0"/>
+        <v>6.9444444444444198E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="37"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="39">
+        <f t="shared" si="2"/>
+        <v>0.36874999999999997</v>
+      </c>
+      <c r="D10" s="39">
+        <f t="shared" si="1"/>
+        <v>0.36944444444444441</v>
+      </c>
+      <c r="E10" s="37">
+        <v>4</v>
+      </c>
+      <c r="F10" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="G10" s="41">
+        <f t="shared" si="0"/>
+        <v>6.9444444444444198E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="37"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="39">
+        <f t="shared" si="2"/>
+        <v>0.37013888888888885</v>
+      </c>
+      <c r="D11" s="39">
+        <f t="shared" si="1"/>
+        <v>0.37083333333333329</v>
+      </c>
+      <c r="E11" s="37">
+        <v>5</v>
+      </c>
+      <c r="F11" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="G11" s="41">
+        <f t="shared" si="0"/>
+        <v>6.9444444444444198E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="37"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="39">
+        <f t="shared" si="2"/>
+        <v>0.37152777777777773</v>
+      </c>
+      <c r="D12" s="39">
+        <f t="shared" si="1"/>
+        <v>0.37222222222222218</v>
+      </c>
+      <c r="E12" s="37">
+        <v>6</v>
+      </c>
+      <c r="F12" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="G12" s="41">
+        <f t="shared" si="0"/>
+        <v>6.9444444444444198E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="37"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="41"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="37"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="41"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="37"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="41"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="37"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="41"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="37"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="41"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="37"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="41"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="42"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="41">
+        <f>SUM(G7:G18)</f>
+        <v>4.1666666666666519E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
@@ -955,7 +1894,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -1343,7 +2282,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -1727,7 +2666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -2007,91 +2946,619 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="8" customWidth="1"/>
+    <col min="5" max="5" width="4.28515625" customWidth="1"/>
+    <col min="6" max="6" width="50.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="44.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="5"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="2">
-        <f>'weeknr 48web'!H31</f>
-        <v>0.1423611111111111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="2">
-        <f>'weeknr 48game'!H31</f>
-        <v>0.18680555555555567</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B9" s="2">
-        <f>'weeknr 49web'!H31</f>
-        <v>4.8611111111110938E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="7">
-        <f>SUM(B7:B8)</f>
-        <v>0.32916666666666677</v>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1">
+        <v>41617</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" s="2">
+        <f>D8-C8</f>
+        <v>1.0416666666666685E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+      <c r="C9" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" ref="H9:H18" si="0">D9-C9</f>
+        <v>1.0416666666666685E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="C10" s="2">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="0"/>
+        <v>1.041666666666663E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="C11" s="2">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.40625</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0416666666666685E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" s="2">
+        <v>0.40625</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0416666666666685E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="C13" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.4201388888888889</v>
+      </c>
+      <c r="E13">
+        <v>6</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="0"/>
+        <v>3.4722222222222099E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="C14" s="2">
+        <v>0.4201388888888889</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="E14">
+        <v>7</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="0"/>
+        <v>2.777777777777779E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="2">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.48888888888888887</v>
+      </c>
+      <c r="E15">
+        <v>8</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="0"/>
+        <v>4.0972222222222188E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="2">
+        <v>0.48888888888888887</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E16">
+        <v>9</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1111111111111127E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="E17">
+        <v>10</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="0"/>
+        <v>1.041666666666663E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18">
+        <v>11</v>
+      </c>
+      <c r="F18" s="9"/>
+      <c r="H18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>5</v>
+      </c>
+      <c r="H31" s="2">
+        <f>SUM(H8:H30)</f>
+        <v>0.14583333333333331</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H31"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="8" customWidth="1"/>
+    <col min="5" max="5" width="4.28515625" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1">
+        <v>41617</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.62152777777777779</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>71</v>
+      </c>
+      <c r="H8" s="2">
+        <f>D8-C8</f>
+        <v>6.9444444444444198E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" ref="H9:H18" si="0">D9-C9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13">
+        <v>6</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14">
+        <v>7</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15">
+        <v>8</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16">
+        <v>9</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17">
+        <v>10</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18">
+        <v>11</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>5</v>
+      </c>
+      <c r="H31" s="2">
+        <f>SUM(H8:H30)</f>
+        <v>6.9444444444444198E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>